<commit_message>
update for ecology submission
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coyotesusd-my.sharepoint.com/personal/jeff_wesner_usd_edu/Documents/USD/Github Projects/stan_isd/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{080DC89D-F11A-4F8E-8FF9-FF016C35A0E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{080DC89D-F11A-4F8E-8FF9-FF016C35A0E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{62E60A7F-60DF-4D09-AE3E-D8AE21498F6D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{4FA5DD8E-B408-4AF4-98D1-ED71BB357598}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="2" xr2:uid="{4FA5DD8E-B408-4AF4-98D1-ED71BB357598}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -92,11 +93,38 @@
   <si>
     <t>Table 2. Slope values from a regression testing the relationship between the ISD exponent and year for IBTS trawl data (Edwards et al. 2020). The values are derived using the Bayesian hierarchical model presented here or from the maximum likelihood approach described in Edwards et al. 2020).</t>
   </si>
+  <si>
+    <t>N(-1.8, 0.01)</t>
+  </si>
+  <si>
+    <t>True lambda</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>N(-1.8, 0.10)</t>
+  </si>
+  <si>
+    <t>N(-1.8, 2.00)</t>
+  </si>
+  <si>
+    <t>Prior(mean, sd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table S1: Prior sensitivity analysis showing how the posterior estimate of lambda changes as the prior standard deviation becomes more restrictive. The posteriors are summarized for models run on the same dataset containing 1000 simulated individuals from a true lambda of -1.98, xmin = 1, and xmax = 1000. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -183,15 +211,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,14 +568,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -803,23 +850,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5B2CC8-243F-415B-9CBE-C4BD068476A1}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="11" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="22.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -853,13 +900,13 @@
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>-1E-3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -871,7 +918,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2476438-1278-4654-938E-40C19773D269}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>-1.98</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="18">
+        <v>-2.0163199365467501</v>
+      </c>
+      <c r="D4" s="18">
+        <v>3.2836529809539099E-2</v>
+      </c>
+      <c r="E4" s="18">
+        <v>-2.0820503743098402</v>
+      </c>
+      <c r="F4" s="18">
+        <v>-1.9563786345238099</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>-1.98</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="18">
+        <v>-2.00872546482874</v>
+      </c>
+      <c r="D5" s="18">
+        <v>3.1534142145203899E-2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>-2.0733016365995001</v>
+      </c>
+      <c r="F5" s="18">
+        <v>-1.94232528076384</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>-1.98</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="19">
+        <v>-1.8639256700214999</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1.6281848994227101E-2</v>
+      </c>
+      <c r="E6" s="19">
+        <v>-1.8968423401739301</v>
+      </c>
+      <c r="F6" s="19">
+        <v>-1.8333993401278199</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010D08B74DB13F641A1FB2572219BFE55" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d72e6b404a86689d5149284bbb843f28">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="26133458-dd6b-4323-9224-444c1d830d6d" xmlns:ns4="ab955a96-761f-4c96-a6fc-04b9ce4c53f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2fd11072b5cff02776c944f38ca4696e" ns3:_="" ns4:_="">
     <xsd:import namespace="26133458-dd6b-4323-9224-444c1d830d6d"/>
@@ -1108,7 +1290,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1117,13 +1299,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B199A2E6-C9AC-4234-987C-1EF22CDD3A38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ab955a96-761f-4c96-a6fc-04b9ce4c53f5"/>
+    <ds:schemaRef ds:uri="26133458-dd6b-4323-9224-444c1d830d6d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81E709DF-760D-4C7E-A296-268709D14F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1142,27 +1335,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B896F199-852F-43A0-BA51-726C7FAA7BA5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B199A2E6-C9AC-4234-987C-1EF22CDD3A38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ab955a96-761f-4c96-a6fc-04b9ce4c53f5"/>
-    <ds:schemaRef ds:uri="26133458-dd6b-4323-9224-444c1d830d6d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>